<commit_message>
Updated s3 file name and fixed tests
</commit_message>
<xml_diff>
--- a/grizly/tests/tables.xlsx
+++ b/grizly/tests/tables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC895E-DEA3-4434-A326-8A820E908117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AACF5A-A5E3-4DE0-BD1E-6F6BE3863923}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,18 +53,12 @@
     <t>column_as</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Order Number</t>
-  </si>
-  <si>
     <t>orders_schema</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>CASE WHEN CustomerID_1 &lt;&gt; NULL THEN CustomerID_1 ELSE CustomerID_2 END</t>
+  </si>
+  <si>
+    <t>Order_Number</t>
+  </si>
+  <si>
+    <t>Order_Nr</t>
   </si>
 </sst>
 </file>
@@ -146,12 +146,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -437,7 +440,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,35 +468,35 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -504,7 +507,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -516,7 +519,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -530,7 +533,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -544,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -591,18 +594,18 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -610,7 +613,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -618,7 +621,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -626,7 +629,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>

</xml_diff>